<commit_message>
update eventloader with new eventtyes
</commit_message>
<xml_diff>
--- a/storage/app/eventbatch.xlsx
+++ b/storage/app/eventbatch.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Eduardo\Desarrollo\home\Eduardo\laravel\cooking-point\storage\app\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{106B5BFA-68D2-4F8A-A4CE-E0C1E3E9AD86}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B20368B-C461-44FD-BFB5-930ADD8567A7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="eventbatch" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">eventbatch!$A$2:$D$32</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">eventbatch!$A$2:$D$155</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="899" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="814" uniqueCount="13">
   <si>
     <t>DIA</t>
   </si>
@@ -53,22 +53,28 @@
     <t>clase2</t>
   </si>
   <si>
-    <t>ONLINE-SELECTION-MORNING</t>
+    <t>ONLINE-MORNING-SELECTION</t>
   </si>
   <si>
-    <t>ONLINE-SELECTION-EVENING</t>
+    <t>ONLINE-EVENING-SELECTION</t>
   </si>
   <si>
-    <t>ONLINE-SELECTION-LATENIGHT</t>
+    <t>ONLINE-LATENIGHT-SELECTION</t>
   </si>
   <si>
-    <t>ONLINE-PAELLA-MORNING</t>
+    <t>ONLINE-LATENIGHT-PAELLA</t>
   </si>
   <si>
-    <t>ONLINE-PAELLA-EVENING</t>
+    <t>ONLINE-MORNING-PAELLA</t>
   </si>
   <si>
-    <t>ONLINE-PAELLA-LATENIGHT</t>
+    <t>ONLINE-EVENING-PAELLA</t>
+  </si>
+  <si>
+    <t>PAELLA</t>
+  </si>
+  <si>
+    <t>TAPAS</t>
   </si>
 </sst>
 </file>
@@ -433,10 +439,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H251"/>
+  <sheetPr filterMode="1"/>
+  <dimension ref="A1:J251"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A156" sqref="A156:XFD251"/>
+    <sheetView tabSelected="1" topLeftCell="A102" workbookViewId="0">
+      <selection activeCell="D123" sqref="D123"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -485,13 +492,13 @@
         <v>7</v>
       </c>
       <c r="F3" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="G3" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="H3" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
@@ -513,13 +520,13 @@
         <v>7</v>
       </c>
       <c r="F4" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="G4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="H4" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
@@ -541,13 +548,13 @@
         <v>7</v>
       </c>
       <c r="F5" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="G5" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="H5" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
@@ -569,13 +576,13 @@
         <v>7</v>
       </c>
       <c r="F6" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="G6" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="H6" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
@@ -597,16 +604,16 @@
         <v>7</v>
       </c>
       <c r="F7" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="G7" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="H7" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A8">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -635,13 +642,13 @@
         <v>7</v>
       </c>
       <c r="F9" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="G9" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="H9" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
@@ -663,13 +670,13 @@
         <v>7</v>
       </c>
       <c r="F10" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="G10" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="H10" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
@@ -691,13 +698,13 @@
         <v>7</v>
       </c>
       <c r="F11" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="G11" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="H11" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
@@ -719,13 +726,13 @@
         <v>7</v>
       </c>
       <c r="F12" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="G12" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="H12" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
@@ -747,13 +754,13 @@
         <v>7</v>
       </c>
       <c r="F13" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="G13" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="H13" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
@@ -775,16 +782,16 @@
         <v>7</v>
       </c>
       <c r="F14" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="G14" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="H14" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A15">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -813,13 +820,13 @@
         <v>7</v>
       </c>
       <c r="F16" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="G16" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="H16" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
@@ -841,13 +848,13 @@
         <v>7</v>
       </c>
       <c r="F17" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="G17" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="H17" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
@@ -869,13 +876,13 @@
         <v>7</v>
       </c>
       <c r="F18" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="G18" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="H18" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
@@ -897,13 +904,13 @@
         <v>7</v>
       </c>
       <c r="F19" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="G19" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="H19" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
@@ -925,13 +932,13 @@
         <v>7</v>
       </c>
       <c r="F20" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="G20" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="H20" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
@@ -953,16 +960,16 @@
         <v>7</v>
       </c>
       <c r="F21" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="G21" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="H21" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A22">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -991,13 +998,13 @@
         <v>7</v>
       </c>
       <c r="F23" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="G23" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="H23" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
@@ -1019,13 +1026,13 @@
         <v>7</v>
       </c>
       <c r="F24" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="G24" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="H24" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
@@ -1047,13 +1054,13 @@
         <v>7</v>
       </c>
       <c r="F25" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="G25" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="H25" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
@@ -1075,13 +1082,13 @@
         <v>7</v>
       </c>
       <c r="F26" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="G26" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="H26" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
@@ -1103,13 +1110,13 @@
         <v>7</v>
       </c>
       <c r="F27" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="G27" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="H27" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
@@ -1131,16 +1138,16 @@
         <v>7</v>
       </c>
       <c r="F28" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="G28" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="H28" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A29">
         <f t="shared" si="2"/>
         <v>7</v>
@@ -1169,13 +1176,13 @@
         <v>7</v>
       </c>
       <c r="F30" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="G30" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="H30" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
@@ -1197,13 +1204,13 @@
         <v>7</v>
       </c>
       <c r="F31" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="G31" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="H31" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
@@ -1225,13 +1232,13 @@
         <v>7</v>
       </c>
       <c r="F32" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="G32" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="H32" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
@@ -1253,13 +1260,13 @@
         <v>7</v>
       </c>
       <c r="F33" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="G33" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="H33" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
@@ -1281,13 +1288,13 @@
         <v>7</v>
       </c>
       <c r="F34" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="G34" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="H34" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.25">
@@ -1309,16 +1316,16 @@
         <v>7</v>
       </c>
       <c r="F35" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="G35" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="H35" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A36">
         <f t="shared" si="3"/>
         <v>7</v>
@@ -1326,24 +1333,6 @@
       <c r="B36" s="1">
         <f t="shared" si="1"/>
         <v>44108</v>
-      </c>
-      <c r="C36" t="s">
-        <v>5</v>
-      </c>
-      <c r="D36" t="s">
-        <v>6</v>
-      </c>
-      <c r="E36" t="s">
-        <v>7</v>
-      </c>
-      <c r="F36" t="s">
-        <v>8</v>
-      </c>
-      <c r="G36" t="s">
-        <v>9</v>
-      </c>
-      <c r="H36" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.25">
@@ -1365,13 +1354,13 @@
         <v>7</v>
       </c>
       <c r="F37" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="G37" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="H37" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.25">
@@ -1393,13 +1382,13 @@
         <v>7</v>
       </c>
       <c r="F38" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="G38" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="H38" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.25">
@@ -1421,13 +1410,13 @@
         <v>7</v>
       </c>
       <c r="F39" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="G39" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="H39" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.25">
@@ -1449,13 +1438,13 @@
         <v>7</v>
       </c>
       <c r="F40" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="G40" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="H40" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.25">
@@ -1477,13 +1466,13 @@
         <v>7</v>
       </c>
       <c r="F41" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="G41" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="H41" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.25">
@@ -1505,16 +1494,16 @@
         <v>7</v>
       </c>
       <c r="F42" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="G42" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="H42" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A43">
         <f t="shared" si="3"/>
         <v>7</v>
@@ -1522,24 +1511,6 @@
       <c r="B43" s="1">
         <f t="shared" si="1"/>
         <v>44115</v>
-      </c>
-      <c r="C43" t="s">
-        <v>5</v>
-      </c>
-      <c r="D43" t="s">
-        <v>6</v>
-      </c>
-      <c r="E43" t="s">
-        <v>7</v>
-      </c>
-      <c r="F43" t="s">
-        <v>8</v>
-      </c>
-      <c r="G43" t="s">
-        <v>9</v>
-      </c>
-      <c r="H43" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.25">
@@ -1561,13 +1532,13 @@
         <v>7</v>
       </c>
       <c r="F44" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="G44" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="H44" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.25">
@@ -1589,13 +1560,13 @@
         <v>7</v>
       </c>
       <c r="F45" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="G45" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="H45" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.25">
@@ -1617,13 +1588,13 @@
         <v>7</v>
       </c>
       <c r="F46" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="G46" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="H46" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.25">
@@ -1645,13 +1616,13 @@
         <v>7</v>
       </c>
       <c r="F47" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="G47" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="H47" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.25">
@@ -1673,13 +1644,13 @@
         <v>7</v>
       </c>
       <c r="F48" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="G48" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="H48" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.25">
@@ -1701,16 +1672,16 @@
         <v>7</v>
       </c>
       <c r="F49" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="G49" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="H49" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A50">
         <f t="shared" si="3"/>
         <v>7</v>
@@ -1718,24 +1689,6 @@
       <c r="B50" s="1">
         <f t="shared" si="1"/>
         <v>44122</v>
-      </c>
-      <c r="C50" t="s">
-        <v>5</v>
-      </c>
-      <c r="D50" t="s">
-        <v>6</v>
-      </c>
-      <c r="E50" t="s">
-        <v>7</v>
-      </c>
-      <c r="F50" t="s">
-        <v>8</v>
-      </c>
-      <c r="G50" t="s">
-        <v>9</v>
-      </c>
-      <c r="H50" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.25">
@@ -1757,13 +1710,13 @@
         <v>7</v>
       </c>
       <c r="F51" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="G51" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="H51" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.25">
@@ -1785,13 +1738,13 @@
         <v>7</v>
       </c>
       <c r="F52" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="G52" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="H52" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.25">
@@ -1813,13 +1766,13 @@
         <v>7</v>
       </c>
       <c r="F53" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="G53" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="H53" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.25">
@@ -1841,13 +1794,13 @@
         <v>7</v>
       </c>
       <c r="F54" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="G54" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="H54" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.25">
@@ -1869,13 +1822,13 @@
         <v>7</v>
       </c>
       <c r="F55" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="G55" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="H55" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.25">
@@ -1897,16 +1850,16 @@
         <v>7</v>
       </c>
       <c r="F56" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="G56" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="H56" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="57" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A57">
         <f t="shared" si="3"/>
         <v>7</v>
@@ -1914,24 +1867,6 @@
       <c r="B57" s="1">
         <f t="shared" si="1"/>
         <v>44129</v>
-      </c>
-      <c r="C57" t="s">
-        <v>5</v>
-      </c>
-      <c r="D57" t="s">
-        <v>6</v>
-      </c>
-      <c r="E57" t="s">
-        <v>7</v>
-      </c>
-      <c r="F57" t="s">
-        <v>8</v>
-      </c>
-      <c r="G57" t="s">
-        <v>9</v>
-      </c>
-      <c r="H57" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="58" spans="1:8" x14ac:dyDescent="0.25">
@@ -1953,13 +1888,13 @@
         <v>7</v>
       </c>
       <c r="F58" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="G58" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="H58" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="59" spans="1:8" x14ac:dyDescent="0.25">
@@ -1981,13 +1916,13 @@
         <v>7</v>
       </c>
       <c r="F59" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="G59" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="H59" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="60" spans="1:8" x14ac:dyDescent="0.25">
@@ -2009,13 +1944,13 @@
         <v>7</v>
       </c>
       <c r="F60" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="G60" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="H60" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="61" spans="1:8" x14ac:dyDescent="0.25">
@@ -2037,13 +1972,13 @@
         <v>7</v>
       </c>
       <c r="F61" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="G61" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="H61" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="62" spans="1:8" x14ac:dyDescent="0.25">
@@ -2065,13 +2000,13 @@
         <v>7</v>
       </c>
       <c r="F62" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="G62" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="H62" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="63" spans="1:8" x14ac:dyDescent="0.25">
@@ -2093,16 +2028,16 @@
         <v>7</v>
       </c>
       <c r="F63" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="G63" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="H63" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="64" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A64">
         <f t="shared" si="3"/>
         <v>7</v>
@@ -2110,24 +2045,6 @@
       <c r="B64" s="1">
         <f t="shared" si="1"/>
         <v>44136</v>
-      </c>
-      <c r="C64" t="s">
-        <v>5</v>
-      </c>
-      <c r="D64" t="s">
-        <v>6</v>
-      </c>
-      <c r="E64" t="s">
-        <v>7</v>
-      </c>
-      <c r="F64" t="s">
-        <v>8</v>
-      </c>
-      <c r="G64" t="s">
-        <v>9</v>
-      </c>
-      <c r="H64" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="65" spans="1:8" x14ac:dyDescent="0.25">
@@ -2149,13 +2066,13 @@
         <v>7</v>
       </c>
       <c r="F65" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="G65" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="H65" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="66" spans="1:8" x14ac:dyDescent="0.25">
@@ -2177,13 +2094,13 @@
         <v>7</v>
       </c>
       <c r="F66" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="G66" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="H66" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="67" spans="1:8" x14ac:dyDescent="0.25">
@@ -2205,13 +2122,13 @@
         <v>7</v>
       </c>
       <c r="F67" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="G67" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="H67" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="68" spans="1:8" x14ac:dyDescent="0.25">
@@ -2233,13 +2150,13 @@
         <v>7</v>
       </c>
       <c r="F68" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="G68" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="H68" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="69" spans="1:8" x14ac:dyDescent="0.25">
@@ -2261,13 +2178,13 @@
         <v>7</v>
       </c>
       <c r="F69" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="G69" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="H69" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="70" spans="1:8" x14ac:dyDescent="0.25">
@@ -2289,16 +2206,16 @@
         <v>7</v>
       </c>
       <c r="F70" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="G70" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="H70" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="71" spans="1:8" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="71" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A71">
         <f t="shared" si="3"/>
         <v>7</v>
@@ -2306,24 +2223,6 @@
       <c r="B71" s="1">
         <f t="shared" si="4"/>
         <v>44143</v>
-      </c>
-      <c r="C71" t="s">
-        <v>5</v>
-      </c>
-      <c r="D71" t="s">
-        <v>6</v>
-      </c>
-      <c r="E71" t="s">
-        <v>7</v>
-      </c>
-      <c r="F71" t="s">
-        <v>8</v>
-      </c>
-      <c r="G71" t="s">
-        <v>9</v>
-      </c>
-      <c r="H71" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="72" spans="1:8" x14ac:dyDescent="0.25">
@@ -2345,13 +2244,13 @@
         <v>7</v>
       </c>
       <c r="F72" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="G72" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="H72" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="73" spans="1:8" x14ac:dyDescent="0.25">
@@ -2373,13 +2272,13 @@
         <v>7</v>
       </c>
       <c r="F73" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="G73" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="H73" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="74" spans="1:8" x14ac:dyDescent="0.25">
@@ -2401,13 +2300,13 @@
         <v>7</v>
       </c>
       <c r="F74" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="G74" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="H74" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="75" spans="1:8" x14ac:dyDescent="0.25">
@@ -2429,13 +2328,13 @@
         <v>7</v>
       </c>
       <c r="F75" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="G75" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="H75" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="76" spans="1:8" x14ac:dyDescent="0.25">
@@ -2457,13 +2356,13 @@
         <v>7</v>
       </c>
       <c r="F76" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="G76" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="H76" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="77" spans="1:8" x14ac:dyDescent="0.25">
@@ -2485,16 +2384,16 @@
         <v>7</v>
       </c>
       <c r="F77" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="G77" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="H77" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="78" spans="1:8" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="78" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A78">
         <f t="shared" si="3"/>
         <v>7</v>
@@ -2502,24 +2401,6 @@
       <c r="B78" s="1">
         <f t="shared" si="4"/>
         <v>44150</v>
-      </c>
-      <c r="C78" t="s">
-        <v>5</v>
-      </c>
-      <c r="D78" t="s">
-        <v>6</v>
-      </c>
-      <c r="E78" t="s">
-        <v>7</v>
-      </c>
-      <c r="F78" t="s">
-        <v>8</v>
-      </c>
-      <c r="G78" t="s">
-        <v>9</v>
-      </c>
-      <c r="H78" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="79" spans="1:8" x14ac:dyDescent="0.25">
@@ -2541,13 +2422,13 @@
         <v>7</v>
       </c>
       <c r="F79" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="G79" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="H79" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="80" spans="1:8" x14ac:dyDescent="0.25">
@@ -2569,13 +2450,13 @@
         <v>7</v>
       </c>
       <c r="F80" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="G80" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="H80" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="81" spans="1:8" x14ac:dyDescent="0.25">
@@ -2597,13 +2478,13 @@
         <v>7</v>
       </c>
       <c r="F81" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="G81" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="H81" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="82" spans="1:8" x14ac:dyDescent="0.25">
@@ -2625,13 +2506,13 @@
         <v>7</v>
       </c>
       <c r="F82" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="G82" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="H82" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="83" spans="1:8" x14ac:dyDescent="0.25">
@@ -2653,13 +2534,13 @@
         <v>7</v>
       </c>
       <c r="F83" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="G83" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="H83" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="84" spans="1:8" x14ac:dyDescent="0.25">
@@ -2681,16 +2562,16 @@
         <v>7</v>
       </c>
       <c r="F84" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="G84" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="H84" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="85" spans="1:8" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="85" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A85">
         <f t="shared" si="3"/>
         <v>7</v>
@@ -2698,24 +2579,6 @@
       <c r="B85" s="1">
         <f t="shared" si="4"/>
         <v>44157</v>
-      </c>
-      <c r="C85" t="s">
-        <v>5</v>
-      </c>
-      <c r="D85" t="s">
-        <v>6</v>
-      </c>
-      <c r="E85" t="s">
-        <v>7</v>
-      </c>
-      <c r="F85" t="s">
-        <v>8</v>
-      </c>
-      <c r="G85" t="s">
-        <v>9</v>
-      </c>
-      <c r="H85" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="86" spans="1:8" x14ac:dyDescent="0.25">
@@ -2737,13 +2600,13 @@
         <v>7</v>
       </c>
       <c r="F86" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="G86" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="H86" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="87" spans="1:8" x14ac:dyDescent="0.25">
@@ -2765,13 +2628,13 @@
         <v>7</v>
       </c>
       <c r="F87" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="G87" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="H87" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="88" spans="1:8" x14ac:dyDescent="0.25">
@@ -2793,13 +2656,13 @@
         <v>7</v>
       </c>
       <c r="F88" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="G88" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="H88" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="89" spans="1:8" x14ac:dyDescent="0.25">
@@ -2821,13 +2684,13 @@
         <v>7</v>
       </c>
       <c r="F89" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="G89" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="H89" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="90" spans="1:8" x14ac:dyDescent="0.25">
@@ -2849,13 +2712,13 @@
         <v>7</v>
       </c>
       <c r="F90" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="G90" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="H90" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="91" spans="1:8" x14ac:dyDescent="0.25">
@@ -2877,16 +2740,16 @@
         <v>7</v>
       </c>
       <c r="F91" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="G91" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="H91" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="92" spans="1:8" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="92" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A92">
         <f t="shared" si="3"/>
         <v>7</v>
@@ -2894,24 +2757,6 @@
       <c r="B92" s="1">
         <f t="shared" si="4"/>
         <v>44164</v>
-      </c>
-      <c r="C92" t="s">
-        <v>5</v>
-      </c>
-      <c r="D92" t="s">
-        <v>6</v>
-      </c>
-      <c r="E92" t="s">
-        <v>7</v>
-      </c>
-      <c r="F92" t="s">
-        <v>8</v>
-      </c>
-      <c r="G92" t="s">
-        <v>9</v>
-      </c>
-      <c r="H92" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="93" spans="1:8" x14ac:dyDescent="0.25">
@@ -2933,13 +2778,13 @@
         <v>7</v>
       </c>
       <c r="F93" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="G93" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="H93" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="94" spans="1:8" x14ac:dyDescent="0.25">
@@ -2961,13 +2806,13 @@
         <v>7</v>
       </c>
       <c r="F94" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="G94" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="H94" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="95" spans="1:8" x14ac:dyDescent="0.25">
@@ -2989,13 +2834,13 @@
         <v>7</v>
       </c>
       <c r="F95" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="G95" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="H95" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="96" spans="1:8" x14ac:dyDescent="0.25">
@@ -3017,18 +2862,18 @@
         <v>7</v>
       </c>
       <c r="F96" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="G96" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="H96" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="97" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A97">
-        <f t="shared" ref="A97:A160" si="5">+WEEKDAY(B97,2)</f>
+        <f t="shared" ref="A97:A155" si="5">+WEEKDAY(B97,2)</f>
         <v>5</v>
       </c>
       <c r="B97" s="1">
@@ -3045,13 +2890,13 @@
         <v>7</v>
       </c>
       <c r="F97" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="G97" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="H97" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="98" spans="1:8" x14ac:dyDescent="0.25">
@@ -3073,16 +2918,16 @@
         <v>7</v>
       </c>
       <c r="F98" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="G98" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="H98" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="99" spans="1:8" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="99" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A99">
         <f t="shared" si="5"/>
         <v>7</v>
@@ -3090,24 +2935,6 @@
       <c r="B99" s="1">
         <f t="shared" si="4"/>
         <v>44171</v>
-      </c>
-      <c r="C99" t="s">
-        <v>5</v>
-      </c>
-      <c r="D99" t="s">
-        <v>6</v>
-      </c>
-      <c r="E99" t="s">
-        <v>7</v>
-      </c>
-      <c r="F99" t="s">
-        <v>8</v>
-      </c>
-      <c r="G99" t="s">
-        <v>9</v>
-      </c>
-      <c r="H99" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="100" spans="1:8" x14ac:dyDescent="0.25">
@@ -3129,13 +2956,13 @@
         <v>7</v>
       </c>
       <c r="F100" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="G100" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="H100" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="101" spans="1:8" x14ac:dyDescent="0.25">
@@ -3157,13 +2984,13 @@
         <v>7</v>
       </c>
       <c r="F101" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="G101" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="H101" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="102" spans="1:8" x14ac:dyDescent="0.25">
@@ -3185,13 +3012,13 @@
         <v>7</v>
       </c>
       <c r="F102" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="G102" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="H102" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="103" spans="1:8" x14ac:dyDescent="0.25">
@@ -3213,13 +3040,13 @@
         <v>7</v>
       </c>
       <c r="F103" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="G103" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="H103" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="104" spans="1:8" x14ac:dyDescent="0.25">
@@ -3241,13 +3068,13 @@
         <v>7</v>
       </c>
       <c r="F104" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="G104" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="H104" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="105" spans="1:8" x14ac:dyDescent="0.25">
@@ -3269,16 +3096,16 @@
         <v>7</v>
       </c>
       <c r="F105" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="G105" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="H105" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="106" spans="1:8" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="106" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A106">
         <f t="shared" si="5"/>
         <v>7</v>
@@ -3286,24 +3113,6 @@
       <c r="B106" s="1">
         <f t="shared" si="4"/>
         <v>44178</v>
-      </c>
-      <c r="C106" t="s">
-        <v>5</v>
-      </c>
-      <c r="D106" t="s">
-        <v>6</v>
-      </c>
-      <c r="E106" t="s">
-        <v>7</v>
-      </c>
-      <c r="F106" t="s">
-        <v>8</v>
-      </c>
-      <c r="G106" t="s">
-        <v>9</v>
-      </c>
-      <c r="H106" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="107" spans="1:8" x14ac:dyDescent="0.25">
@@ -3325,13 +3134,13 @@
         <v>7</v>
       </c>
       <c r="F107" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="G107" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="H107" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="108" spans="1:8" x14ac:dyDescent="0.25">
@@ -3353,13 +3162,13 @@
         <v>7</v>
       </c>
       <c r="F108" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="G108" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="H108" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="109" spans="1:8" x14ac:dyDescent="0.25">
@@ -3381,13 +3190,13 @@
         <v>7</v>
       </c>
       <c r="F109" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="G109" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="H109" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="110" spans="1:8" x14ac:dyDescent="0.25">
@@ -3409,13 +3218,13 @@
         <v>7</v>
       </c>
       <c r="F110" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="G110" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="H110" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="111" spans="1:8" x14ac:dyDescent="0.25">
@@ -3437,13 +3246,13 @@
         <v>7</v>
       </c>
       <c r="F111" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="G111" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="H111" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="112" spans="1:8" x14ac:dyDescent="0.25">
@@ -3465,16 +3274,16 @@
         <v>7</v>
       </c>
       <c r="F112" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="G112" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="H112" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="113" spans="1:8" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="113" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A113">
         <f t="shared" si="5"/>
         <v>7</v>
@@ -3483,26 +3292,8 @@
         <f t="shared" si="4"/>
         <v>44185</v>
       </c>
-      <c r="C113" t="s">
-        <v>5</v>
-      </c>
-      <c r="D113" t="s">
-        <v>6</v>
-      </c>
-      <c r="E113" t="s">
-        <v>7</v>
-      </c>
-      <c r="F113" t="s">
-        <v>8</v>
-      </c>
-      <c r="G113" t="s">
-        <v>9</v>
-      </c>
-      <c r="H113" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="114" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="114" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A114">
         <f t="shared" si="5"/>
         <v>1</v>
@@ -3521,16 +3312,16 @@
         <v>7</v>
       </c>
       <c r="F114" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="G114" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="H114" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="115" spans="1:8" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="115" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A115">
         <f t="shared" si="5"/>
         <v>2</v>
@@ -3549,16 +3340,16 @@
         <v>7</v>
       </c>
       <c r="F115" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="G115" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="H115" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="116" spans="1:8" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="116" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A116">
         <f t="shared" si="5"/>
         <v>3</v>
@@ -3577,16 +3368,16 @@
         <v>7</v>
       </c>
       <c r="F116" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="G116" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="H116" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="117" spans="1:8" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="117" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A117">
         <f t="shared" si="5"/>
         <v>4</v>
@@ -3595,26 +3386,8 @@
         <f t="shared" si="4"/>
         <v>44189</v>
       </c>
-      <c r="C117" t="s">
-        <v>5</v>
-      </c>
-      <c r="D117" t="s">
-        <v>6</v>
-      </c>
-      <c r="E117" t="s">
-        <v>7</v>
-      </c>
-      <c r="F117" t="s">
-        <v>8</v>
-      </c>
-      <c r="G117" t="s">
-        <v>9</v>
-      </c>
-      <c r="H117" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="118" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="118" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A118">
         <f t="shared" si="5"/>
         <v>5</v>
@@ -3623,26 +3396,8 @@
         <f t="shared" si="4"/>
         <v>44190</v>
       </c>
-      <c r="C118" t="s">
-        <v>5</v>
-      </c>
-      <c r="D118" t="s">
-        <v>6</v>
-      </c>
-      <c r="E118" t="s">
-        <v>7</v>
-      </c>
-      <c r="F118" t="s">
-        <v>8</v>
-      </c>
-      <c r="G118" t="s">
-        <v>9</v>
-      </c>
-      <c r="H118" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="119" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="119" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A119">
         <f t="shared" si="5"/>
         <v>6</v>
@@ -3661,16 +3416,16 @@
         <v>7</v>
       </c>
       <c r="F119" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="G119" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="H119" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="120" spans="1:8" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="120" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A120">
         <f t="shared" si="5"/>
         <v>7</v>
@@ -3679,26 +3434,8 @@
         <f t="shared" si="4"/>
         <v>44192</v>
       </c>
-      <c r="C120" t="s">
-        <v>5</v>
-      </c>
-      <c r="D120" t="s">
-        <v>6</v>
-      </c>
-      <c r="E120" t="s">
-        <v>7</v>
-      </c>
-      <c r="F120" t="s">
-        <v>8</v>
-      </c>
-      <c r="G120" t="s">
-        <v>9</v>
-      </c>
-      <c r="H120" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="121" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="121" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A121">
         <f t="shared" si="5"/>
         <v>1</v>
@@ -3717,16 +3454,16 @@
         <v>7</v>
       </c>
       <c r="F121" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="G121" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="H121" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="122" spans="1:8" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="122" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A122">
         <f t="shared" si="5"/>
         <v>2</v>
@@ -3745,16 +3482,16 @@
         <v>7</v>
       </c>
       <c r="F122" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="G122" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="H122" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="123" spans="1:8" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="123" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A123">
         <f t="shared" si="5"/>
         <v>3</v>
@@ -3773,16 +3510,16 @@
         <v>7</v>
       </c>
       <c r="F123" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="G123" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="H123" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="124" spans="1:8" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="124" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A124">
         <f t="shared" si="5"/>
         <v>4</v>
@@ -3801,16 +3538,16 @@
         <v>7</v>
       </c>
       <c r="F124" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="G124" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="H124" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="125" spans="1:8" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="125" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A125">
         <f t="shared" si="5"/>
         <v>5</v>
@@ -3819,26 +3556,8 @@
         <f t="shared" si="4"/>
         <v>44197</v>
       </c>
-      <c r="C125" t="s">
-        <v>5</v>
-      </c>
-      <c r="D125" t="s">
-        <v>6</v>
-      </c>
-      <c r="E125" t="s">
-        <v>7</v>
-      </c>
-      <c r="F125" t="s">
-        <v>8</v>
-      </c>
-      <c r="G125" t="s">
-        <v>9</v>
-      </c>
-      <c r="H125" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="126" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="126" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A126">
         <f t="shared" si="5"/>
         <v>6</v>
@@ -3847,26 +3566,8 @@
         <f t="shared" si="4"/>
         <v>44198</v>
       </c>
-      <c r="C126" t="s">
-        <v>5</v>
-      </c>
-      <c r="D126" t="s">
-        <v>6</v>
-      </c>
-      <c r="E126" t="s">
-        <v>7</v>
-      </c>
-      <c r="F126" t="s">
-        <v>8</v>
-      </c>
-      <c r="G126" t="s">
-        <v>9</v>
-      </c>
-      <c r="H126" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="127" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="127" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A127">
         <f t="shared" si="5"/>
         <v>7</v>
@@ -3875,26 +3576,8 @@
         <f t="shared" si="4"/>
         <v>44199</v>
       </c>
-      <c r="C127" t="s">
-        <v>5</v>
-      </c>
-      <c r="D127" t="s">
-        <v>6</v>
-      </c>
-      <c r="E127" t="s">
-        <v>7</v>
-      </c>
-      <c r="F127" t="s">
-        <v>8</v>
-      </c>
-      <c r="G127" t="s">
-        <v>9</v>
-      </c>
-      <c r="H127" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="128" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="128" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A128">
         <f t="shared" si="5"/>
         <v>1</v>
@@ -3913,16 +3596,22 @@
         <v>7</v>
       </c>
       <c r="F128" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="G128" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="H128" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="129" spans="1:8" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+      <c r="I128" t="s">
+        <v>11</v>
+      </c>
+      <c r="J128" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="129" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A129">
         <f t="shared" si="5"/>
         <v>2</v>
@@ -3941,16 +3630,22 @@
         <v>7</v>
       </c>
       <c r="F129" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="G129" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="H129" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="130" spans="1:8" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+      <c r="I129" t="s">
+        <v>11</v>
+      </c>
+      <c r="J129" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="130" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A130">
         <f t="shared" si="5"/>
         <v>3</v>
@@ -3969,16 +3664,22 @@
         <v>7</v>
       </c>
       <c r="F130" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="G130" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="H130" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="131" spans="1:8" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+      <c r="I130" t="s">
+        <v>11</v>
+      </c>
+      <c r="J130" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="131" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A131">
         <f t="shared" si="5"/>
         <v>4</v>
@@ -3997,16 +3698,22 @@
         <v>7</v>
       </c>
       <c r="F131" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="G131" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="H131" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="132" spans="1:8" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+      <c r="I131" t="s">
+        <v>11</v>
+      </c>
+      <c r="J131" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="132" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A132">
         <f t="shared" si="5"/>
         <v>5</v>
@@ -4025,22 +3732,28 @@
         <v>7</v>
       </c>
       <c r="F132" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="G132" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="H132" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="133" spans="1:8" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+      <c r="I132" t="s">
+        <v>11</v>
+      </c>
+      <c r="J132" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="133" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A133">
         <f t="shared" si="5"/>
         <v>6</v>
       </c>
       <c r="B133" s="1">
-        <f t="shared" ref="B133:B196" si="6">+B132+1</f>
+        <f t="shared" ref="B133:B155" si="6">+B132+1</f>
         <v>44205</v>
       </c>
       <c r="C133" t="s">
@@ -4053,16 +3766,19 @@
         <v>7</v>
       </c>
       <c r="F133" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="G133" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="H133" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="134" spans="1:8" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+      <c r="I133" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="134" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A134">
         <f t="shared" si="5"/>
         <v>7</v>
@@ -4071,26 +3787,8 @@
         <f t="shared" si="6"/>
         <v>44206</v>
       </c>
-      <c r="C134" t="s">
-        <v>5</v>
-      </c>
-      <c r="D134" t="s">
-        <v>6</v>
-      </c>
-      <c r="E134" t="s">
-        <v>7</v>
-      </c>
-      <c r="F134" t="s">
-        <v>8</v>
-      </c>
-      <c r="G134" t="s">
-        <v>9</v>
-      </c>
-      <c r="H134" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="135" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="135" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A135">
         <f t="shared" si="5"/>
         <v>1</v>
@@ -4109,16 +3807,22 @@
         <v>7</v>
       </c>
       <c r="F135" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="G135" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="H135" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="136" spans="1:8" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+      <c r="I135" t="s">
+        <v>11</v>
+      </c>
+      <c r="J135" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="136" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A136">
         <f t="shared" si="5"/>
         <v>2</v>
@@ -4137,16 +3841,22 @@
         <v>7</v>
       </c>
       <c r="F136" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="G136" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="H136" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="137" spans="1:8" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+      <c r="I136" t="s">
+        <v>11</v>
+      </c>
+      <c r="J136" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="137" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A137">
         <f t="shared" si="5"/>
         <v>3</v>
@@ -4165,16 +3875,22 @@
         <v>7</v>
       </c>
       <c r="F137" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="G137" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="H137" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="138" spans="1:8" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+      <c r="I137" t="s">
+        <v>11</v>
+      </c>
+      <c r="J137" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="138" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A138">
         <f t="shared" si="5"/>
         <v>4</v>
@@ -4193,16 +3909,22 @@
         <v>7</v>
       </c>
       <c r="F138" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="G138" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="H138" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="139" spans="1:8" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+      <c r="I138" t="s">
+        <v>11</v>
+      </c>
+      <c r="J138" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="139" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A139">
         <f t="shared" si="5"/>
         <v>5</v>
@@ -4221,16 +3943,22 @@
         <v>7</v>
       </c>
       <c r="F139" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="G139" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="H139" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="140" spans="1:8" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+      <c r="I139" t="s">
+        <v>11</v>
+      </c>
+      <c r="J139" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="140" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A140">
         <f t="shared" si="5"/>
         <v>6</v>
@@ -4249,16 +3977,22 @@
         <v>7</v>
       </c>
       <c r="F140" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="G140" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="H140" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="141" spans="1:8" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+      <c r="I140" t="s">
+        <v>11</v>
+      </c>
+      <c r="J140" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="141" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A141">
         <f t="shared" si="5"/>
         <v>7</v>
@@ -4267,26 +4001,8 @@
         <f t="shared" si="6"/>
         <v>44213</v>
       </c>
-      <c r="C141" t="s">
-        <v>5</v>
-      </c>
-      <c r="D141" t="s">
-        <v>6</v>
-      </c>
-      <c r="E141" t="s">
-        <v>7</v>
-      </c>
-      <c r="F141" t="s">
-        <v>8</v>
-      </c>
-      <c r="G141" t="s">
-        <v>9</v>
-      </c>
-      <c r="H141" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="142" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="142" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A142">
         <f t="shared" si="5"/>
         <v>1</v>
@@ -4305,16 +4021,22 @@
         <v>7</v>
       </c>
       <c r="F142" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="G142" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="H142" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="143" spans="1:8" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+      <c r="I142" t="s">
+        <v>11</v>
+      </c>
+      <c r="J142" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="143" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A143">
         <f t="shared" si="5"/>
         <v>2</v>
@@ -4333,16 +4055,22 @@
         <v>7</v>
       </c>
       <c r="F143" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="G143" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="H143" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="144" spans="1:8" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+      <c r="I143" t="s">
+        <v>11</v>
+      </c>
+      <c r="J143" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="144" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A144">
         <f t="shared" si="5"/>
         <v>3</v>
@@ -4361,16 +4089,22 @@
         <v>7</v>
       </c>
       <c r="F144" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="G144" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="H144" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="145" spans="1:8" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+      <c r="I144" t="s">
+        <v>11</v>
+      </c>
+      <c r="J144" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="145" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A145">
         <f t="shared" si="5"/>
         <v>4</v>
@@ -4389,16 +4123,22 @@
         <v>7</v>
       </c>
       <c r="F145" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="G145" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="H145" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="146" spans="1:8" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+      <c r="I145" t="s">
+        <v>11</v>
+      </c>
+      <c r="J145" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="146" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A146">
         <f t="shared" si="5"/>
         <v>5</v>
@@ -4417,16 +4157,22 @@
         <v>7</v>
       </c>
       <c r="F146" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="G146" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="H146" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="147" spans="1:8" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+      <c r="I146" t="s">
+        <v>11</v>
+      </c>
+      <c r="J146" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="147" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A147">
         <f t="shared" si="5"/>
         <v>6</v>
@@ -4445,16 +4191,22 @@
         <v>7</v>
       </c>
       <c r="F147" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="G147" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="H147" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="148" spans="1:8" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+      <c r="I147" t="s">
+        <v>11</v>
+      </c>
+      <c r="J147" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="148" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A148">
         <f t="shared" si="5"/>
         <v>7</v>
@@ -4463,26 +4215,8 @@
         <f t="shared" si="6"/>
         <v>44220</v>
       </c>
-      <c r="C148" t="s">
-        <v>5</v>
-      </c>
-      <c r="D148" t="s">
-        <v>6</v>
-      </c>
-      <c r="E148" t="s">
-        <v>7</v>
-      </c>
-      <c r="F148" t="s">
-        <v>8</v>
-      </c>
-      <c r="G148" t="s">
-        <v>9</v>
-      </c>
-      <c r="H148" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="149" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="149" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A149">
         <f t="shared" si="5"/>
         <v>1</v>
@@ -4501,16 +4235,22 @@
         <v>7</v>
       </c>
       <c r="F149" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="G149" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="H149" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="150" spans="1:8" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+      <c r="I149" t="s">
+        <v>11</v>
+      </c>
+      <c r="J149" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="150" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A150">
         <f t="shared" si="5"/>
         <v>2</v>
@@ -4529,16 +4269,22 @@
         <v>7</v>
       </c>
       <c r="F150" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="G150" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="H150" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="151" spans="1:8" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+      <c r="I150" t="s">
+        <v>11</v>
+      </c>
+      <c r="J150" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="151" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A151">
         <f t="shared" si="5"/>
         <v>3</v>
@@ -4557,16 +4303,22 @@
         <v>7</v>
       </c>
       <c r="F151" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="G151" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="H151" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="152" spans="1:8" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+      <c r="I151" t="s">
+        <v>11</v>
+      </c>
+      <c r="J151" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="152" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A152">
         <f t="shared" si="5"/>
         <v>4</v>
@@ -4585,16 +4337,22 @@
         <v>7</v>
       </c>
       <c r="F152" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="G152" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="H152" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="153" spans="1:8" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+      <c r="I152" t="s">
+        <v>11</v>
+      </c>
+      <c r="J152" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="153" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A153">
         <f t="shared" si="5"/>
         <v>5</v>
@@ -4613,16 +4371,22 @@
         <v>7</v>
       </c>
       <c r="F153" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="G153" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="H153" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="154" spans="1:8" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+      <c r="I153" t="s">
+        <v>11</v>
+      </c>
+      <c r="J153" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="154" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A154">
         <f t="shared" si="5"/>
         <v>6</v>
@@ -4641,16 +4405,22 @@
         <v>7</v>
       </c>
       <c r="F154" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="G154" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="H154" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="155" spans="1:8" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+      <c r="I154" t="s">
+        <v>11</v>
+      </c>
+      <c r="J154" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="155" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A155">
         <f t="shared" si="5"/>
         <v>7</v>
@@ -4659,38 +4429,20 @@
         <f t="shared" si="6"/>
         <v>44227</v>
       </c>
-      <c r="C155" t="s">
-        <v>5</v>
-      </c>
-      <c r="D155" t="s">
-        <v>6</v>
-      </c>
-      <c r="E155" t="s">
-        <v>7</v>
-      </c>
-      <c r="F155" t="s">
-        <v>8</v>
-      </c>
-      <c r="G155" t="s">
-        <v>9</v>
-      </c>
-      <c r="H155" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="156" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="156" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B156" s="1"/>
     </row>
-    <row r="157" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B157" s="1"/>
     </row>
-    <row r="158" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B158" s="1"/>
     </row>
-    <row r="159" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B159" s="1"/>
     </row>
-    <row r="160" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B160" s="1"/>
     </row>
     <row r="161" spans="2:2" x14ac:dyDescent="0.25">
@@ -4967,7 +4719,18 @@
       <c r="B251" s="1"/>
     </row>
   </sheetData>
-  <autoFilter ref="A2:D32" xr:uid="{96A57D41-D021-40F2-9509-6A286A85AB4D}"/>
+  <autoFilter ref="A2:D155" xr:uid="{96A57D41-D021-40F2-9509-6A286A85AB4D}">
+    <filterColumn colId="0">
+      <filters>
+        <filter val="1"/>
+        <filter val="2"/>
+        <filter val="3"/>
+        <filter val="4"/>
+        <filter val="5"/>
+        <filter val="6"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <mergeCells count="1">
     <mergeCell ref="A1:D1"/>
   </mergeCells>

</xml_diff>